<commit_message>
* decrease loop_exec list
</commit_message>
<xml_diff>
--- a/evaluation/loop_exec_option.xlsx
+++ b/evaluation/loop_exec_option.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="27">
   <si>
     <t xml:space="preserve">branch_name</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/isshy-you/tetris.git</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ish05g6</t>
   </si>
   <si>
     <t xml:space="preserve">refer</t>
@@ -249,11 +246,11 @@
   </sheetPr>
   <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.11"/>
@@ -3580,822 +3577,298 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B86" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C86" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D86" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F86" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H86" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I86" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J86" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K86" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L86" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A86" s="3"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="3"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
+      <c r="L86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B87" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C87" s="5" t="n">
-        <f aca="false">seed_list!$B$2</f>
-        <v>620</v>
-      </c>
-      <c r="D87" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F87" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H87" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I87" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K87" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L87" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A87" s="3"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="3"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="3"/>
+      <c r="K87" s="3"/>
+      <c r="L87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B88" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C88" s="5" t="n">
-        <f aca="false">seed_list!$B$3</f>
-        <v>149</v>
-      </c>
-      <c r="D88" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F88" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H88" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I88" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K88" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L88" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A88" s="3"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3"/>
+      <c r="L88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B89" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C89" s="5" t="n">
-        <f aca="false">seed_list!$B$4</f>
-        <v>48</v>
-      </c>
-      <c r="D89" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F89" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H89" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I89" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L89" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A89" s="3"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="5"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3"/>
+      <c r="L89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B90" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C90" s="5" t="n">
-        <f aca="false">seed_list!$B$5</f>
-        <v>270</v>
-      </c>
-      <c r="D90" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F90" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H90" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I90" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J90" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K90" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L90" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A90" s="3"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="6"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B91" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C91" s="5" t="n">
-        <f aca="false">seed_list!$B$6</f>
-        <v>714</v>
-      </c>
-      <c r="D91" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F91" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H91" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I91" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J91" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K91" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L91" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A91" s="3"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="6"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B92" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C92" s="5" t="n">
-        <f aca="false">seed_list!$B$7</f>
-        <v>339</v>
-      </c>
-      <c r="D92" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F92" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H92" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I92" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J92" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K92" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L92" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A92" s="3"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="6"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B93" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C93" s="5" t="n">
-        <f aca="false">seed_list!$B$8</f>
-        <v>240</v>
-      </c>
-      <c r="D93" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E93" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F93" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H93" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I93" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J93" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K93" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L93" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A93" s="3"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+      <c r="L93" s="6"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B94" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C94" s="5" t="n">
-        <f aca="false">seed_list!$B$9</f>
-        <v>804</v>
-      </c>
-      <c r="D94" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F94" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H94" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I94" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J94" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K94" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L94" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A94" s="3"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="5"/>
+      <c r="I94" s="5"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B95" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C95" s="5" t="n">
-        <f aca="false">seed_list!$B$10</f>
-        <v>531</v>
-      </c>
-      <c r="D95" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F95" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H95" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I95" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J95" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K95" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L95" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A95" s="3"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B96" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C96" s="5" t="n">
-        <f aca="false">seed_list!$B$11</f>
-        <v>348</v>
-      </c>
-      <c r="D96" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F96" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H96" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I96" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J96" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K96" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L96" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A96" s="3"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="3"/>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
+      <c r="J96" s="3"/>
+      <c r="K96" s="3"/>
+      <c r="L96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B97" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C97" s="5" t="n">
-        <f aca="false">seed_list!$B$2</f>
-        <v>620</v>
-      </c>
-      <c r="D97" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F97" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H97" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I97" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J97" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K97" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L97" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A97" s="3"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="3"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="3"/>
+      <c r="K97" s="3"/>
+      <c r="L97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B98" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C98" s="5" t="n">
-        <f aca="false">seed_list!$B$3</f>
-        <v>149</v>
-      </c>
-      <c r="D98" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F98" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H98" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I98" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J98" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K98" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L98" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A98" s="3"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="3"/>
+      <c r="K98" s="3"/>
+      <c r="L98" s="6"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B99" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C99" s="5" t="n">
-        <f aca="false">seed_list!$B$4</f>
-        <v>48</v>
-      </c>
-      <c r="D99" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F99" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H99" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I99" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J99" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K99" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L99" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A99" s="3"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B100" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C100" s="5" t="n">
-        <f aca="false">seed_list!$B$5</f>
-        <v>270</v>
-      </c>
-      <c r="D100" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F100" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H100" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I100" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K100" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L100" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A100" s="3"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B101" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C101" s="5" t="n">
-        <f aca="false">seed_list!$B$6</f>
-        <v>714</v>
-      </c>
-      <c r="D101" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F101" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H101" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I101" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K101" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L101" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A101" s="3"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="5"/>
+      <c r="I101" s="5"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+      <c r="L101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B102" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C102" s="5" t="n">
-        <f aca="false">seed_list!$B$7</f>
-        <v>339</v>
-      </c>
-      <c r="D102" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F102" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H102" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I102" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J102" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K102" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L102" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A102" s="3"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="5"/>
+      <c r="I102" s="5"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="6"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B103" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C103" s="5" t="n">
-        <f aca="false">seed_list!$B$8</f>
-        <v>240</v>
-      </c>
-      <c r="D103" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F103" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H103" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I103" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L103" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A103" s="3"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="6"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B104" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C104" s="5" t="n">
-        <f aca="false">seed_list!$B$9</f>
-        <v>804</v>
-      </c>
-      <c r="D104" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F104" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H104" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I104" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J104" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K104" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L104" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A104" s="3"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="6"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B105" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C105" s="5" t="n">
-        <f aca="false">seed_list!$B$10</f>
-        <v>531</v>
-      </c>
-      <c r="D105" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F105" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H105" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I105" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J105" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K105" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L105" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A105" s="3"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="6"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B106" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="C106" s="5" t="n">
-        <f aca="false">seed_list!$B$11</f>
-        <v>348</v>
-      </c>
-      <c r="D106" s="5" t="n">
-        <v>180</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F106" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H106" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I106" s="5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K106" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L106" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A106" s="3"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3"/>
@@ -5007,18 +4480,18 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,7 +4507,7 @@
       </c>
       <c r="D2" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>857</v>
+        <v>986</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +4523,7 @@
       </c>
       <c r="D3" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>401</v>
+        <v>956</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5066,7 +4539,7 @@
       </c>
       <c r="D4" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>43</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5082,7 +4555,7 @@
       </c>
       <c r="D5" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>386</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5098,7 +4571,7 @@
       </c>
       <c r="D6" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>967</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5114,7 +4587,7 @@
       </c>
       <c r="D7" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5130,7 +4603,7 @@
       </c>
       <c r="D8" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5146,7 +4619,7 @@
       </c>
       <c r="D9" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>634</v>
+        <v>534</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5162,7 +4635,7 @@
       </c>
       <c r="D10" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>936</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5178,7 +4651,7 @@
       </c>
       <c r="D11" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>321</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* update evaluation to latest seigot/master
</commit_message>
<xml_diff>
--- a/evaluation/loop_exec_option.xlsx
+++ b/evaluation/loop_exec_option.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">REPOSITORY</t>
   </si>
   <si>
-    <t xml:space="preserve">ish06b</t>
+    <t xml:space="preserve">ish08a</t>
   </si>
   <si>
     <t xml:space="preserve">default</t>
@@ -229,10 +229,10 @@
   <dimension ref="A1:L64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.11"/>
@@ -312,7 +312,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>15</v>
@@ -351,7 +351,7 @@
         <v>6</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>15</v>
@@ -390,7 +390,7 @@
         <v>6</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>15</v>
@@ -429,7 +429,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>15</v>
@@ -468,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>15</v>
@@ -507,7 +507,7 @@
         <v>6</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>15</v>
@@ -546,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>15</v>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>15</v>
@@ -624,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>15</v>
@@ -663,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>15</v>
@@ -702,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>15</v>
@@ -741,7 +741,7 @@
         <v>6</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>15</v>
@@ -780,7 +780,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>15</v>
@@ -819,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>15</v>
@@ -858,7 +858,7 @@
         <v>6</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>15</v>
@@ -897,7 +897,7 @@
         <v>6</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>15</v>
@@ -936,7 +936,7 @@
         <v>6</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>15</v>
@@ -975,7 +975,7 @@
         <v>6</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>15</v>
@@ -1014,7 +1014,7 @@
         <v>6</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>15</v>
@@ -1053,7 +1053,7 @@
         <v>6</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>15</v>
@@ -1092,7 +1092,7 @@
         <v>6</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>1000</v>
+        <v>180</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>15</v>
@@ -1714,7 +1714,7 @@
       <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="D2" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>815</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="D3" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>283</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="D4" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>471</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="D5" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>813</v>
+        <v>634</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="D6" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>198</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="D7" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>673</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D8" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>6</v>
+        <v>929</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="D9" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>862</v>
+        <v>560</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="D10" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>25</v>
+        <v>796</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="D11" s="5" t="n">
         <f aca="false">com.sun.star.sheet.addin.Analysis.getRandbetween(1,999)</f>
-        <v>988</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>